<commit_message>
Exclude BEVs from local air pollution
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_TRA_Emissions.xlsx
+++ b/SuppXLS/Scen_B_TRA_Emissions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\~g2v_TIM\TRA_VA6\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A47E08-BF45-4D31-AAA1-D206FF3323D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1BFA26-B1DA-4922-B95F-E8900E2778DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="2316" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="15" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1650" uniqueCount="453">
   <si>
     <t>Pset_CI</t>
   </si>
@@ -1505,13 +1505,16 @@
     <t>Mopeds</t>
   </si>
   <si>
-    <t>T-LGT*</t>
-  </si>
-  <si>
-    <t>T-MGT*,T-HGT*</t>
-  </si>
-  <si>
     <t>Light trucks</t>
+  </si>
+  <si>
+    <t>T-BUS*,-T-BUS-BEV*</t>
+  </si>
+  <si>
+    <t>T-MGT*,T-HGT*,-T-MGT-BEV*,-T-HGT-BEV*</t>
+  </si>
+  <si>
+    <t>T-LGT*,-T-LGT-BEV*</t>
   </si>
 </sst>
 </file>
@@ -2103,6 +2106,8 @@
     <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2130,8 +2135,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma 2" xfId="3" xr:uid="{AB97AD92-C767-4954-8EC7-D9D8F846878E}"/>
@@ -4192,8 +4195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{776C821D-D078-45D4-B6B7-4704861B2C88}">
   <dimension ref="A2:M95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5167,7 +5170,7 @@
     </row>
     <row r="46" spans="1:12" s="95" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="46" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
@@ -5178,12 +5181,12 @@
         <v>80</v>
       </c>
       <c r="H46" s="86" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="I46" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="K46" s="114">
+      <c r="K46" s="105">
         <v>0</v>
       </c>
       <c r="L46" s="102" t="s">
@@ -5200,7 +5203,7 @@
         <v>80</v>
       </c>
       <c r="H47" s="86" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="I47" s="95" t="s">
         <v>83</v>
@@ -5224,7 +5227,7 @@
         <v>80</v>
       </c>
       <c r="H48" s="86" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="I48" s="95" t="s">
         <v>81</v>
@@ -5249,7 +5252,7 @@
         <v>80</v>
       </c>
       <c r="H49" s="45" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="I49" s="43" t="s">
         <v>86</v>
@@ -5273,12 +5276,12 @@
         <v>80</v>
       </c>
       <c r="H50" s="86" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I50" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="K50" s="114">
+      <c r="K50" s="105">
         <v>0</v>
       </c>
       <c r="L50" s="102" t="s">
@@ -5295,7 +5298,7 @@
         <v>80</v>
       </c>
       <c r="H51" s="86" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I51" s="95" t="s">
         <v>83</v>
@@ -5317,7 +5320,7 @@
         <v>80</v>
       </c>
       <c r="H52" s="86" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I52" s="95" t="s">
         <v>81</v>
@@ -5342,7 +5345,7 @@
         <v>80</v>
       </c>
       <c r="H53" s="45" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I53" s="43" t="s">
         <v>86</v>
@@ -5367,13 +5370,13 @@
         <v>80</v>
       </c>
       <c r="H54" s="86" t="s">
-        <v>162</v>
+        <v>450</v>
       </c>
       <c r="I54" s="95" t="s">
         <v>82</v>
       </c>
       <c r="J54" s="86"/>
-      <c r="K54" s="113">
+      <c r="K54" s="104">
         <v>0</v>
       </c>
       <c r="L54" s="102" t="s">
@@ -5391,7 +5394,7 @@
         <v>80</v>
       </c>
       <c r="H55" s="86" t="s">
-        <v>162</v>
+        <v>450</v>
       </c>
       <c r="I55" s="95" t="s">
         <v>83</v>
@@ -5417,7 +5420,7 @@
         <v>80</v>
       </c>
       <c r="H56" s="86" t="s">
-        <v>162</v>
+        <v>450</v>
       </c>
       <c r="I56" s="95" t="s">
         <v>81</v>
@@ -5443,7 +5446,7 @@
         <v>80</v>
       </c>
       <c r="H57" s="45" t="s">
-        <v>162</v>
+        <v>450</v>
       </c>
       <c r="I57" s="43" t="s">
         <v>86</v>
@@ -6043,10 +6046,10 @@
       <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="B3" s="108"/>
+      <c r="B3" s="110"/>
       <c r="C3" s="14"/>
       <c r="D3" s="21" t="s">
         <v>92</v>
@@ -6074,7 +6077,7 @@
       <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="107" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="22" t="s">
@@ -6115,7 +6118,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A5" s="106"/>
+      <c r="A5" s="108"/>
       <c r="B5" s="25"/>
       <c r="C5" s="14"/>
       <c r="D5" s="23" t="s">
@@ -6138,7 +6141,7 @@
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="14"/>
-      <c r="L5" s="104" t="s">
+      <c r="L5" s="106" t="s">
         <v>101</v>
       </c>
       <c r="M5" s="42" t="s">
@@ -6150,7 +6153,7 @@
       <c r="O5" s="42"/>
     </row>
     <row r="6" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A6" s="106"/>
+      <c r="A6" s="108"/>
       <c r="B6" s="25"/>
       <c r="C6" s="14"/>
       <c r="D6" s="23" t="s">
@@ -6173,7 +6176,7 @@
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
-      <c r="L6" s="104"/>
+      <c r="L6" s="106"/>
       <c r="M6" s="42" t="s">
         <v>105</v>
       </c>
@@ -6183,7 +6186,7 @@
       <c r="O6" s="42"/>
     </row>
     <row r="7" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A7" s="106"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="25"/>
       <c r="C7" s="19" t="s">
         <v>82</v>
@@ -6208,7 +6211,7 @@
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="14"/>
-      <c r="L7" s="104"/>
+      <c r="L7" s="106"/>
       <c r="M7" s="42" t="s">
         <v>107</v>
       </c>
@@ -6218,7 +6221,7 @@
       <c r="O7" s="42"/>
     </row>
     <row r="8" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A8" s="106"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="25"/>
       <c r="C8" s="19" t="s">
         <v>83</v>
@@ -6243,7 +6246,7 @@
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="14"/>
-      <c r="L8" s="104"/>
+      <c r="L8" s="106"/>
       <c r="M8" s="42" t="s">
         <v>108</v>
       </c>
@@ -6253,7 +6256,7 @@
       <c r="O8" s="42"/>
     </row>
     <row r="9" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A9" s="106"/>
+      <c r="A9" s="108"/>
       <c r="B9" s="25"/>
       <c r="C9" s="19" t="s">
         <v>84</v>
@@ -6278,7 +6281,7 @@
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
-      <c r="L9" s="104"/>
+      <c r="L9" s="106"/>
       <c r="M9" s="42" t="s">
         <v>110</v>
       </c>
@@ -6288,7 +6291,7 @@
       <c r="O9" s="42"/>
     </row>
     <row r="10" spans="1:15" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A10" s="106"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="25"/>
       <c r="C10" s="19" t="s">
         <v>85</v>
@@ -6313,7 +6316,7 @@
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
-      <c r="L10" s="104"/>
+      <c r="L10" s="106"/>
       <c r="M10" s="42" t="s">
         <v>112</v>
       </c>
@@ -6323,7 +6326,7 @@
       <c r="O10" s="42"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="106"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="27" t="s">
         <v>113</v>
       </c>
@@ -6354,7 +6357,7 @@
       <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="106"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="31"/>
       <c r="C12" s="14"/>
       <c r="D12" s="28" t="s">
@@ -6383,7 +6386,7 @@
       <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="106"/>
+      <c r="A13" s="108"/>
       <c r="B13" s="31"/>
       <c r="C13" s="14"/>
       <c r="D13" s="28" t="s">
@@ -6412,7 +6415,7 @@
       <c r="O13" s="14"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="106"/>
+      <c r="A14" s="108"/>
       <c r="B14" s="31"/>
       <c r="C14" s="19" t="s">
         <v>82</v>
@@ -6451,7 +6454,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="106"/>
+      <c r="A15" s="108"/>
       <c r="B15" s="31"/>
       <c r="C15" s="19" t="s">
         <v>83</v>
@@ -6476,7 +6479,7 @@
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="104" t="s">
+      <c r="L15" s="106" t="s">
         <v>114</v>
       </c>
       <c r="M15" s="42" t="s">
@@ -6488,7 +6491,7 @@
       <c r="O15" s="42"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="106"/>
+      <c r="A16" s="108"/>
       <c r="B16" s="31"/>
       <c r="C16" s="19" t="s">
         <v>84</v>
@@ -6513,7 +6516,7 @@
       </c>
       <c r="J16" s="14"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="104"/>
+      <c r="L16" s="106"/>
       <c r="M16" s="42" t="s">
         <v>105</v>
       </c>
@@ -6523,7 +6526,7 @@
       <c r="O16" s="42"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="106"/>
+      <c r="A17" s="108"/>
       <c r="B17" s="31"/>
       <c r="C17" s="19" t="s">
         <v>85</v>
@@ -6548,7 +6551,7 @@
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="14"/>
-      <c r="L17" s="104"/>
+      <c r="L17" s="106"/>
       <c r="M17" s="42" t="s">
         <v>107</v>
       </c>
@@ -6558,7 +6561,7 @@
       <c r="O17" s="42"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="106"/>
+      <c r="A18" s="108"/>
       <c r="B18" s="22" t="s">
         <v>115</v>
       </c>
@@ -6583,7 +6586,7 @@
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="14"/>
-      <c r="L18" s="104"/>
+      <c r="L18" s="106"/>
       <c r="M18" s="42" t="s">
         <v>108</v>
       </c>
@@ -6593,7 +6596,7 @@
       <c r="O18" s="42"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="106"/>
+      <c r="A19" s="108"/>
       <c r="B19" s="25"/>
       <c r="C19" s="14"/>
       <c r="D19" s="23" t="s">
@@ -6616,7 +6619,7 @@
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="14"/>
-      <c r="L19" s="104"/>
+      <c r="L19" s="106"/>
       <c r="M19" s="42" t="s">
         <v>110</v>
       </c>
@@ -6626,7 +6629,7 @@
       <c r="O19" s="42"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="106"/>
+      <c r="A20" s="108"/>
       <c r="B20" s="25"/>
       <c r="C20" s="14"/>
       <c r="D20" s="23" t="s">
@@ -6649,7 +6652,7 @@
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="14"/>
-      <c r="L20" s="104"/>
+      <c r="L20" s="106"/>
       <c r="M20" s="42" t="s">
         <v>112</v>
       </c>
@@ -6659,7 +6662,7 @@
       <c r="O20" s="42"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="106"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="25"/>
       <c r="C21" s="19" t="s">
         <v>82</v>
@@ -6690,7 +6693,7 @@
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="106"/>
+      <c r="A22" s="108"/>
       <c r="B22" s="25"/>
       <c r="C22" s="19" t="s">
         <v>83</v>
@@ -6721,7 +6724,7 @@
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="106"/>
+      <c r="A23" s="108"/>
       <c r="B23" s="25"/>
       <c r="C23" s="19" t="s">
         <v>84</v>
@@ -6752,7 +6755,7 @@
       <c r="O23" s="14"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="106"/>
+      <c r="A24" s="108"/>
       <c r="B24" s="25"/>
       <c r="C24" s="19" t="s">
         <v>85</v>
@@ -6783,7 +6786,7 @@
       <c r="O24" s="14"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="106"/>
+      <c r="A25" s="108"/>
       <c r="B25" s="27" t="s">
         <v>116</v>
       </c>
@@ -6814,7 +6817,7 @@
       <c r="O25" s="14"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="106"/>
+      <c r="A26" s="108"/>
       <c r="B26" s="31"/>
       <c r="C26" s="14"/>
       <c r="D26" s="28" t="s">
@@ -6843,7 +6846,7 @@
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="106"/>
+      <c r="A27" s="108"/>
       <c r="B27" s="31"/>
       <c r="C27" s="14"/>
       <c r="D27" s="28" t="s">
@@ -6872,7 +6875,7 @@
       <c r="O27" s="14"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="106"/>
+      <c r="A28" s="108"/>
       <c r="B28" s="31"/>
       <c r="C28" s="19" t="s">
         <v>82</v>
@@ -6903,7 +6906,7 @@
       <c r="O28" s="14"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="106"/>
+      <c r="A29" s="108"/>
       <c r="B29" s="31"/>
       <c r="C29" s="19" t="s">
         <v>83</v>
@@ -6934,7 +6937,7 @@
       <c r="O29" s="14"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="106"/>
+      <c r="A30" s="108"/>
       <c r="B30" s="31"/>
       <c r="C30" s="19" t="s">
         <v>84</v>
@@ -6965,7 +6968,7 @@
       <c r="O30" s="14"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A31" s="106"/>
+      <c r="A31" s="108"/>
       <c r="B31" s="31"/>
       <c r="C31" s="19" t="s">
         <v>85</v>
@@ -6996,7 +6999,7 @@
       <c r="O31" s="14"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="106"/>
+      <c r="A32" s="108"/>
       <c r="B32" s="22" t="s">
         <v>117</v>
       </c>
@@ -7027,7 +7030,7 @@
       <c r="O32" s="14"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="106"/>
+      <c r="A33" s="108"/>
       <c r="B33" s="25"/>
       <c r="C33" s="14"/>
       <c r="D33" s="23" t="s">
@@ -7050,7 +7053,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="106"/>
+      <c r="A34" s="108"/>
       <c r="B34" s="25"/>
       <c r="C34" s="14"/>
       <c r="D34" s="23" t="s">
@@ -7073,7 +7076,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="106"/>
+      <c r="A35" s="108"/>
       <c r="B35" s="25"/>
       <c r="C35" s="19" t="s">
         <v>82</v>
@@ -7098,7 +7101,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="106"/>
+      <c r="A36" s="108"/>
       <c r="B36" s="25"/>
       <c r="C36" s="19" t="s">
         <v>83</v>
@@ -7123,7 +7126,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="106"/>
+      <c r="A37" s="108"/>
       <c r="B37" s="25"/>
       <c r="C37" s="19" t="s">
         <v>84</v>
@@ -7148,7 +7151,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="106"/>
+      <c r="A38" s="108"/>
       <c r="B38" s="25"/>
       <c r="C38" s="19" t="s">
         <v>85</v>
@@ -7173,7 +7176,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="106"/>
+      <c r="A39" s="108"/>
       <c r="B39" s="27" t="s">
         <v>118</v>
       </c>
@@ -7198,7 +7201,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="106"/>
+      <c r="A40" s="108"/>
       <c r="B40" s="31"/>
       <c r="C40" s="14"/>
       <c r="D40" s="28" t="s">
@@ -7221,7 +7224,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="106"/>
+      <c r="A41" s="108"/>
       <c r="B41" s="31"/>
       <c r="C41" s="14"/>
       <c r="D41" s="28" t="s">
@@ -7244,7 +7247,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="106"/>
+      <c r="A42" s="108"/>
       <c r="B42" s="31"/>
       <c r="C42" s="19" t="s">
         <v>82</v>
@@ -7269,7 +7272,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="106"/>
+      <c r="A43" s="108"/>
       <c r="B43" s="31"/>
       <c r="C43" s="19" t="s">
         <v>83</v>
@@ -7294,7 +7297,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="106"/>
+      <c r="A44" s="108"/>
       <c r="B44" s="31"/>
       <c r="C44" s="19" t="s">
         <v>84</v>
@@ -7319,7 +7322,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="106"/>
+      <c r="A45" s="108"/>
       <c r="B45" s="31"/>
       <c r="C45" s="19" t="s">
         <v>85</v>
@@ -7344,7 +7347,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="106"/>
+      <c r="A46" s="108"/>
       <c r="B46" s="22" t="s">
         <v>119</v>
       </c>
@@ -7369,7 +7372,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="106"/>
+      <c r="A47" s="108"/>
       <c r="B47" s="25"/>
       <c r="C47" s="14"/>
       <c r="D47" s="23" t="s">
@@ -7392,7 +7395,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="106"/>
+      <c r="A48" s="108"/>
       <c r="B48" s="25"/>
       <c r="C48" s="14"/>
       <c r="D48" s="23" t="s">
@@ -7415,7 +7418,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="106"/>
+      <c r="A49" s="108"/>
       <c r="B49" s="25"/>
       <c r="C49" s="19" t="s">
         <v>82</v>
@@ -7440,7 +7443,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="106"/>
+      <c r="A50" s="108"/>
       <c r="B50" s="25"/>
       <c r="C50" s="19" t="s">
         <v>83</v>
@@ -7465,7 +7468,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="106"/>
+      <c r="A51" s="108"/>
       <c r="B51" s="25"/>
       <c r="C51" s="19" t="s">
         <v>84</v>
@@ -7490,7 +7493,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="106"/>
+      <c r="A52" s="108"/>
       <c r="B52" s="25"/>
       <c r="C52" s="19" t="s">
         <v>85</v>
@@ -7515,7 +7518,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="106"/>
+      <c r="A53" s="108"/>
       <c r="B53" s="27" t="s">
         <v>120</v>
       </c>
@@ -7540,7 +7543,7 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="106"/>
+      <c r="A54" s="108"/>
       <c r="B54" s="31"/>
       <c r="C54" s="14"/>
       <c r="D54" s="28" t="s">
@@ -7563,7 +7566,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="106"/>
+      <c r="A55" s="108"/>
       <c r="B55" s="31"/>
       <c r="C55" s="14"/>
       <c r="D55" s="28" t="s">
@@ -7586,7 +7589,7 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="106"/>
+      <c r="A56" s="108"/>
       <c r="B56" s="31"/>
       <c r="C56" s="19" t="s">
         <v>82</v>
@@ -7611,7 +7614,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="106"/>
+      <c r="A57" s="108"/>
       <c r="B57" s="31"/>
       <c r="C57" s="19" t="s">
         <v>83</v>
@@ -7636,7 +7639,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="106"/>
+      <c r="A58" s="108"/>
       <c r="B58" s="31"/>
       <c r="C58" s="19" t="s">
         <v>84</v>
@@ -7661,7 +7664,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="106"/>
+      <c r="A59" s="108"/>
       <c r="B59" s="31"/>
       <c r="C59" s="19" t="s">
         <v>85</v>
@@ -7686,7 +7689,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="106"/>
+      <c r="A60" s="108"/>
       <c r="B60" s="22" t="s">
         <v>121</v>
       </c>
@@ -7711,7 +7714,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="106"/>
+      <c r="A61" s="108"/>
       <c r="B61" s="25"/>
       <c r="C61" s="14"/>
       <c r="D61" s="23" t="s">
@@ -7734,7 +7737,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="106"/>
+      <c r="A62" s="108"/>
       <c r="B62" s="25"/>
       <c r="C62" s="14"/>
       <c r="D62" s="23" t="s">
@@ -7757,7 +7760,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="106"/>
+      <c r="A63" s="108"/>
       <c r="B63" s="25"/>
       <c r="C63" s="19" t="s">
         <v>82</v>
@@ -7782,7 +7785,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="106"/>
+      <c r="A64" s="108"/>
       <c r="B64" s="25"/>
       <c r="C64" s="19" t="s">
         <v>83</v>
@@ -7807,7 +7810,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="106"/>
+      <c r="A65" s="108"/>
       <c r="B65" s="25"/>
       <c r="C65" s="19" t="s">
         <v>84</v>
@@ -7832,7 +7835,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="106"/>
+      <c r="A66" s="108"/>
       <c r="B66" s="25"/>
       <c r="C66" s="19" t="s">
         <v>85</v>
@@ -7857,7 +7860,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="106"/>
+      <c r="A67" s="108"/>
       <c r="B67" s="27" t="s">
         <v>122</v>
       </c>
@@ -7882,7 +7885,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="106"/>
+      <c r="A68" s="108"/>
       <c r="B68" s="31"/>
       <c r="C68" s="14"/>
       <c r="D68" s="28" t="s">
@@ -7905,7 +7908,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="106"/>
+      <c r="A69" s="108"/>
       <c r="B69" s="31"/>
       <c r="C69" s="14"/>
       <c r="D69" s="28" t="s">
@@ -7928,7 +7931,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="106"/>
+      <c r="A70" s="108"/>
       <c r="B70" s="31"/>
       <c r="C70" s="19" t="s">
         <v>82</v>
@@ -7953,7 +7956,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="106"/>
+      <c r="A71" s="108"/>
       <c r="B71" s="31"/>
       <c r="C71" s="19" t="s">
         <v>83</v>
@@ -7978,7 +7981,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="106"/>
+      <c r="A72" s="108"/>
       <c r="B72" s="31"/>
       <c r="C72" s="19" t="s">
         <v>84</v>
@@ -8003,7 +8006,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="106"/>
+      <c r="A73" s="108"/>
       <c r="B73" s="31"/>
       <c r="C73" s="19" t="s">
         <v>85</v>
@@ -8028,7 +8031,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="106"/>
+      <c r="A74" s="108"/>
       <c r="B74" s="22" t="s">
         <v>123</v>
       </c>
@@ -8053,7 +8056,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="106"/>
+      <c r="A75" s="108"/>
       <c r="B75" s="25"/>
       <c r="C75" s="14"/>
       <c r="D75" s="23" t="s">
@@ -8076,7 +8079,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="106"/>
+      <c r="A76" s="108"/>
       <c r="B76" s="25"/>
       <c r="C76" s="14"/>
       <c r="D76" s="23" t="s">
@@ -8099,7 +8102,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="106"/>
+      <c r="A77" s="108"/>
       <c r="B77" s="25"/>
       <c r="C77" s="19" t="s">
         <v>82</v>
@@ -8124,7 +8127,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="106"/>
+      <c r="A78" s="108"/>
       <c r="B78" s="25"/>
       <c r="C78" s="19" t="s">
         <v>83</v>
@@ -8149,7 +8152,7 @@
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="106"/>
+      <c r="A79" s="108"/>
       <c r="B79" s="25"/>
       <c r="C79" s="19" t="s">
         <v>84</v>
@@ -8174,7 +8177,7 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="106"/>
+      <c r="A80" s="108"/>
       <c r="B80" s="25"/>
       <c r="C80" s="19" t="s">
         <v>85</v>
@@ -8199,7 +8202,7 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="106"/>
+      <c r="A81" s="108"/>
       <c r="B81" s="27" t="s">
         <v>124</v>
       </c>
@@ -8224,7 +8227,7 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="106"/>
+      <c r="A82" s="108"/>
       <c r="B82" s="31"/>
       <c r="C82" s="14"/>
       <c r="D82" s="28" t="s">
@@ -8247,7 +8250,7 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="106"/>
+      <c r="A83" s="108"/>
       <c r="B83" s="31"/>
       <c r="C83" s="14"/>
       <c r="D83" s="28" t="s">
@@ -8270,7 +8273,7 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="106"/>
+      <c r="A84" s="108"/>
       <c r="B84" s="31"/>
       <c r="C84" s="19" t="s">
         <v>82</v>
@@ -8295,7 +8298,7 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="106"/>
+      <c r="A85" s="108"/>
       <c r="B85" s="31"/>
       <c r="C85" s="19" t="s">
         <v>83</v>
@@ -8320,7 +8323,7 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="106"/>
+      <c r="A86" s="108"/>
       <c r="B86" s="31"/>
       <c r="C86" s="19" t="s">
         <v>84</v>
@@ -8345,7 +8348,7 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="106"/>
+      <c r="A87" s="108"/>
       <c r="B87" s="31"/>
       <c r="C87" s="19" t="s">
         <v>85</v>
@@ -8370,7 +8373,7 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="106"/>
+      <c r="A88" s="108"/>
       <c r="B88" s="22" t="s">
         <v>125</v>
       </c>
@@ -8395,7 +8398,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="106"/>
+      <c r="A89" s="108"/>
       <c r="B89" s="25"/>
       <c r="C89" s="14"/>
       <c r="D89" s="23" t="s">
@@ -8418,7 +8421,7 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="106"/>
+      <c r="A90" s="108"/>
       <c r="B90" s="25"/>
       <c r="C90" s="14"/>
       <c r="D90" s="23" t="s">
@@ -8441,7 +8444,7 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="106"/>
+      <c r="A91" s="108"/>
       <c r="B91" s="25"/>
       <c r="C91" s="19" t="s">
         <v>82</v>
@@ -8466,7 +8469,7 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="106"/>
+      <c r="A92" s="108"/>
       <c r="B92" s="25"/>
       <c r="C92" s="19" t="s">
         <v>83</v>
@@ -8491,7 +8494,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="106"/>
+      <c r="A93" s="108"/>
       <c r="B93" s="25"/>
       <c r="C93" s="19" t="s">
         <v>84</v>
@@ -8516,7 +8519,7 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="106"/>
+      <c r="A94" s="108"/>
       <c r="B94" s="25"/>
       <c r="C94" s="19" t="s">
         <v>85</v>
@@ -8541,7 +8544,7 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="106"/>
+      <c r="A95" s="108"/>
       <c r="B95" s="27" t="s">
         <v>126</v>
       </c>
@@ -8566,7 +8569,7 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="106"/>
+      <c r="A96" s="108"/>
       <c r="B96" s="31"/>
       <c r="C96" s="14"/>
       <c r="D96" s="28" t="s">
@@ -8589,7 +8592,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="106"/>
+      <c r="A97" s="108"/>
       <c r="B97" s="31"/>
       <c r="C97" s="14"/>
       <c r="D97" s="28" t="s">
@@ -8612,7 +8615,7 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="106"/>
+      <c r="A98" s="108"/>
       <c r="B98" s="31"/>
       <c r="C98" s="19" t="s">
         <v>82</v>
@@ -8637,7 +8640,7 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="106"/>
+      <c r="A99" s="108"/>
       <c r="B99" s="31"/>
       <c r="C99" s="19" t="s">
         <v>83</v>
@@ -8662,7 +8665,7 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="106"/>
+      <c r="A100" s="108"/>
       <c r="B100" s="31"/>
       <c r="C100" s="19" t="s">
         <v>84</v>
@@ -8687,7 +8690,7 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="106"/>
+      <c r="A101" s="108"/>
       <c r="B101" s="31"/>
       <c r="C101" s="19" t="s">
         <v>85</v>
@@ -8712,7 +8715,7 @@
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="106"/>
+      <c r="A102" s="108"/>
       <c r="B102" s="22" t="s">
         <v>127</v>
       </c>
@@ -8737,7 +8740,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="106"/>
+      <c r="A103" s="108"/>
       <c r="B103" s="25"/>
       <c r="C103" s="14"/>
       <c r="D103" s="23" t="s">
@@ -8760,7 +8763,7 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="106"/>
+      <c r="A104" s="108"/>
       <c r="B104" s="25"/>
       <c r="C104" s="14"/>
       <c r="D104" s="23" t="s">
@@ -8783,7 +8786,7 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="106"/>
+      <c r="A105" s="108"/>
       <c r="B105" s="25"/>
       <c r="C105" s="19" t="s">
         <v>82</v>
@@ -8808,7 +8811,7 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="106"/>
+      <c r="A106" s="108"/>
       <c r="B106" s="25"/>
       <c r="C106" s="19" t="s">
         <v>83</v>
@@ -8833,7 +8836,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="106"/>
+      <c r="A107" s="108"/>
       <c r="B107" s="25"/>
       <c r="C107" s="19" t="s">
         <v>84</v>
@@ -8858,7 +8861,7 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="106"/>
+      <c r="A108" s="108"/>
       <c r="B108" s="25"/>
       <c r="C108" s="19" t="s">
         <v>85</v>
@@ -8883,7 +8886,7 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="106"/>
+      <c r="A109" s="108"/>
       <c r="B109" s="27" t="s">
         <v>128</v>
       </c>
@@ -8908,7 +8911,7 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="106"/>
+      <c r="A110" s="108"/>
       <c r="B110" s="31"/>
       <c r="C110" s="14"/>
       <c r="D110" s="28" t="s">
@@ -8931,7 +8934,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="106"/>
+      <c r="A111" s="108"/>
       <c r="B111" s="31"/>
       <c r="C111" s="14"/>
       <c r="D111" s="28" t="s">
@@ -8954,7 +8957,7 @@
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="106"/>
+      <c r="A112" s="108"/>
       <c r="B112" s="31"/>
       <c r="C112" s="19" t="s">
         <v>82</v>
@@ -8979,7 +8982,7 @@
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="106"/>
+      <c r="A113" s="108"/>
       <c r="B113" s="31"/>
       <c r="C113" s="19" t="s">
         <v>83</v>
@@ -9004,7 +9007,7 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="106"/>
+      <c r="A114" s="108"/>
       <c r="B114" s="31"/>
       <c r="C114" s="19" t="s">
         <v>84</v>
@@ -9029,7 +9032,7 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="106"/>
+      <c r="A115" s="108"/>
       <c r="B115" s="31"/>
       <c r="C115" s="19" t="s">
         <v>85</v>
@@ -9054,7 +9057,7 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="109" t="s">
+      <c r="A116" s="111" t="s">
         <v>129</v>
       </c>
       <c r="B116" s="33" t="s">
@@ -9081,7 +9084,7 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="110"/>
+      <c r="A117" s="112"/>
       <c r="B117" s="36"/>
       <c r="C117" s="14"/>
       <c r="D117" s="34" t="s">
@@ -9104,7 +9107,7 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="110"/>
+      <c r="A118" s="112"/>
       <c r="B118" s="36"/>
       <c r="C118" s="14"/>
       <c r="D118" s="34" t="s">
@@ -9127,7 +9130,7 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="110"/>
+      <c r="A119" s="112"/>
       <c r="B119" s="36"/>
       <c r="C119" s="19" t="s">
         <v>82</v>
@@ -9152,7 +9155,7 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="110"/>
+      <c r="A120" s="112"/>
       <c r="B120" s="36"/>
       <c r="C120" s="19" t="s">
         <v>83</v>
@@ -9177,7 +9180,7 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="110"/>
+      <c r="A121" s="112"/>
       <c r="B121" s="36"/>
       <c r="C121" s="19" t="s">
         <v>84</v>
@@ -9202,7 +9205,7 @@
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="110"/>
+      <c r="A122" s="112"/>
       <c r="B122" s="36"/>
       <c r="C122" s="19" t="s">
         <v>85</v>
@@ -9227,7 +9230,7 @@
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="110"/>
+      <c r="A123" s="112"/>
       <c r="B123" s="37" t="s">
         <v>95</v>
       </c>
@@ -9252,7 +9255,7 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="110"/>
+      <c r="A124" s="112"/>
       <c r="B124" s="40"/>
       <c r="C124" s="14"/>
       <c r="D124" s="38" t="s">
@@ -9275,7 +9278,7 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="110"/>
+      <c r="A125" s="112"/>
       <c r="B125" s="40"/>
       <c r="C125" s="14"/>
       <c r="D125" s="38" t="s">
@@ -9298,7 +9301,7 @@
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="110"/>
+      <c r="A126" s="112"/>
       <c r="B126" s="40"/>
       <c r="C126" s="19" t="s">
         <v>82</v>
@@ -9323,7 +9326,7 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A127" s="110"/>
+      <c r="A127" s="112"/>
       <c r="B127" s="40"/>
       <c r="C127" s="19" t="s">
         <v>83</v>
@@ -9348,7 +9351,7 @@
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="110"/>
+      <c r="A128" s="112"/>
       <c r="B128" s="40"/>
       <c r="C128" s="19" t="s">
         <v>84</v>
@@ -9373,7 +9376,7 @@
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" s="110"/>
+      <c r="A129" s="112"/>
       <c r="B129" s="40"/>
       <c r="C129" s="19" t="s">
         <v>85</v>
@@ -9398,7 +9401,7 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="110"/>
+      <c r="A130" s="112"/>
       <c r="B130" s="33" t="s">
         <v>116</v>
       </c>
@@ -9423,7 +9426,7 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" s="110"/>
+      <c r="A131" s="112"/>
       <c r="B131" s="36"/>
       <c r="C131" s="14"/>
       <c r="D131" s="34" t="s">
@@ -9446,7 +9449,7 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" s="110"/>
+      <c r="A132" s="112"/>
       <c r="B132" s="36"/>
       <c r="C132" s="14"/>
       <c r="D132" s="34" t="s">
@@ -9469,7 +9472,7 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="110"/>
+      <c r="A133" s="112"/>
       <c r="B133" s="36"/>
       <c r="C133" s="19" t="s">
         <v>82</v>
@@ -9494,7 +9497,7 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" s="110"/>
+      <c r="A134" s="112"/>
       <c r="B134" s="36"/>
       <c r="C134" s="19" t="s">
         <v>83</v>
@@ -9519,7 +9522,7 @@
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A135" s="110"/>
+      <c r="A135" s="112"/>
       <c r="B135" s="36"/>
       <c r="C135" s="19" t="s">
         <v>84</v>
@@ -9544,7 +9547,7 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A136" s="110"/>
+      <c r="A136" s="112"/>
       <c r="B136" s="36"/>
       <c r="C136" s="19" t="s">
         <v>85</v>
@@ -9569,7 +9572,7 @@
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A137" s="110"/>
+      <c r="A137" s="112"/>
       <c r="B137" s="37" t="s">
         <v>117</v>
       </c>
@@ -9594,7 +9597,7 @@
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A138" s="110"/>
+      <c r="A138" s="112"/>
       <c r="B138" s="40"/>
       <c r="C138" s="14"/>
       <c r="D138" s="38" t="s">
@@ -9617,7 +9620,7 @@
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A139" s="110"/>
+      <c r="A139" s="112"/>
       <c r="B139" s="40"/>
       <c r="C139" s="14"/>
       <c r="D139" s="38" t="s">
@@ -9640,7 +9643,7 @@
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A140" s="110"/>
+      <c r="A140" s="112"/>
       <c r="B140" s="40"/>
       <c r="C140" s="19" t="s">
         <v>82</v>
@@ -9665,7 +9668,7 @@
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A141" s="110"/>
+      <c r="A141" s="112"/>
       <c r="B141" s="40"/>
       <c r="C141" s="19" t="s">
         <v>83</v>
@@ -9690,7 +9693,7 @@
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" s="110"/>
+      <c r="A142" s="112"/>
       <c r="B142" s="40"/>
       <c r="C142" s="19" t="s">
         <v>84</v>
@@ -9715,7 +9718,7 @@
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A143" s="110"/>
+      <c r="A143" s="112"/>
       <c r="B143" s="40"/>
       <c r="C143" s="19" t="s">
         <v>85</v>
@@ -9740,7 +9743,7 @@
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A144" s="110"/>
+      <c r="A144" s="112"/>
       <c r="B144" s="33" t="s">
         <v>119</v>
       </c>
@@ -9765,7 +9768,7 @@
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A145" s="110"/>
+      <c r="A145" s="112"/>
       <c r="B145" s="36"/>
       <c r="C145" s="14"/>
       <c r="D145" s="34" t="s">
@@ -9788,7 +9791,7 @@
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A146" s="110"/>
+      <c r="A146" s="112"/>
       <c r="B146" s="36"/>
       <c r="C146" s="14"/>
       <c r="D146" s="34" t="s">
@@ -9811,7 +9814,7 @@
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A147" s="110"/>
+      <c r="A147" s="112"/>
       <c r="B147" s="36"/>
       <c r="C147" s="19" t="s">
         <v>82</v>
@@ -9836,7 +9839,7 @@
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A148" s="110"/>
+      <c r="A148" s="112"/>
       <c r="B148" s="36"/>
       <c r="C148" s="19" t="s">
         <v>83</v>
@@ -9861,7 +9864,7 @@
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A149" s="110"/>
+      <c r="A149" s="112"/>
       <c r="B149" s="36"/>
       <c r="C149" s="19" t="s">
         <v>84</v>
@@ -9886,7 +9889,7 @@
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A150" s="110"/>
+      <c r="A150" s="112"/>
       <c r="B150" s="36"/>
       <c r="C150" s="19" t="s">
         <v>85</v>
@@ -9911,7 +9914,7 @@
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A151" s="110"/>
+      <c r="A151" s="112"/>
       <c r="B151" s="37" t="s">
         <v>120</v>
       </c>
@@ -9936,7 +9939,7 @@
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A152" s="110"/>
+      <c r="A152" s="112"/>
       <c r="B152" s="40"/>
       <c r="C152" s="14"/>
       <c r="D152" s="38" t="s">
@@ -9959,7 +9962,7 @@
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A153" s="110"/>
+      <c r="A153" s="112"/>
       <c r="B153" s="40"/>
       <c r="C153" s="14"/>
       <c r="D153" s="38" t="s">
@@ -9982,7 +9985,7 @@
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A154" s="110"/>
+      <c r="A154" s="112"/>
       <c r="B154" s="40"/>
       <c r="C154" s="19" t="s">
         <v>82</v>
@@ -10007,7 +10010,7 @@
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A155" s="110"/>
+      <c r="A155" s="112"/>
       <c r="B155" s="40"/>
       <c r="C155" s="19" t="s">
         <v>83</v>
@@ -10032,7 +10035,7 @@
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A156" s="110"/>
+      <c r="A156" s="112"/>
       <c r="B156" s="40"/>
       <c r="C156" s="19" t="s">
         <v>84</v>
@@ -10057,7 +10060,7 @@
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A157" s="110"/>
+      <c r="A157" s="112"/>
       <c r="B157" s="40"/>
       <c r="C157" s="19" t="s">
         <v>85</v>
@@ -10082,7 +10085,7 @@
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A158" s="110"/>
+      <c r="A158" s="112"/>
       <c r="B158" s="33" t="s">
         <v>123</v>
       </c>
@@ -10107,7 +10110,7 @@
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A159" s="110"/>
+      <c r="A159" s="112"/>
       <c r="B159" s="36"/>
       <c r="C159" s="14"/>
       <c r="D159" s="34" t="s">
@@ -10130,7 +10133,7 @@
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A160" s="110"/>
+      <c r="A160" s="112"/>
       <c r="B160" s="36"/>
       <c r="C160" s="14"/>
       <c r="D160" s="34" t="s">
@@ -10153,7 +10156,7 @@
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A161" s="110"/>
+      <c r="A161" s="112"/>
       <c r="B161" s="36"/>
       <c r="C161" s="19" t="s">
         <v>82</v>
@@ -10178,7 +10181,7 @@
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A162" s="110"/>
+      <c r="A162" s="112"/>
       <c r="B162" s="36"/>
       <c r="C162" s="19" t="s">
         <v>83</v>
@@ -10203,7 +10206,7 @@
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A163" s="110"/>
+      <c r="A163" s="112"/>
       <c r="B163" s="36"/>
       <c r="C163" s="19" t="s">
         <v>84</v>
@@ -10228,7 +10231,7 @@
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A164" s="110"/>
+      <c r="A164" s="112"/>
       <c r="B164" s="36"/>
       <c r="C164" s="19" t="s">
         <v>85</v>
@@ -10253,7 +10256,7 @@
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A165" s="110"/>
+      <c r="A165" s="112"/>
       <c r="B165" s="37" t="s">
         <v>128</v>
       </c>
@@ -10278,7 +10281,7 @@
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A166" s="110"/>
+      <c r="A166" s="112"/>
       <c r="B166" s="40"/>
       <c r="C166" s="14"/>
       <c r="D166" s="38" t="s">
@@ -10301,7 +10304,7 @@
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A167" s="110"/>
+      <c r="A167" s="112"/>
       <c r="B167" s="40"/>
       <c r="C167" s="14"/>
       <c r="D167" s="38" t="s">
@@ -10324,7 +10327,7 @@
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A168" s="110"/>
+      <c r="A168" s="112"/>
       <c r="B168" s="40"/>
       <c r="C168" s="19" t="s">
         <v>82</v>
@@ -10349,7 +10352,7 @@
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A169" s="110"/>
+      <c r="A169" s="112"/>
       <c r="B169" s="40"/>
       <c r="C169" s="19" t="s">
         <v>83</v>
@@ -10374,7 +10377,7 @@
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A170" s="110"/>
+      <c r="A170" s="112"/>
       <c r="B170" s="40"/>
       <c r="C170" s="19" t="s">
         <v>84</v>
@@ -10399,7 +10402,7 @@
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A171" s="110"/>
+      <c r="A171" s="112"/>
       <c r="B171" s="40"/>
       <c r="C171" s="19" t="s">
         <v>85</v>
@@ -10424,7 +10427,7 @@
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A172" s="105" t="s">
+      <c r="A172" s="107" t="s">
         <v>131</v>
       </c>
       <c r="B172" s="22" t="s">
@@ -10451,7 +10454,7 @@
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A173" s="106"/>
+      <c r="A173" s="108"/>
       <c r="B173" s="25"/>
       <c r="C173" s="14"/>
       <c r="D173" s="23" t="s">
@@ -10474,7 +10477,7 @@
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A174" s="106"/>
+      <c r="A174" s="108"/>
       <c r="B174" s="25"/>
       <c r="C174" s="14"/>
       <c r="D174" s="23" t="s">
@@ -10497,7 +10500,7 @@
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A175" s="106"/>
+      <c r="A175" s="108"/>
       <c r="B175" s="25"/>
       <c r="C175" s="19" t="s">
         <v>82</v>
@@ -10522,7 +10525,7 @@
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A176" s="106"/>
+      <c r="A176" s="108"/>
       <c r="B176" s="25"/>
       <c r="C176" s="19" t="s">
         <v>83</v>
@@ -10547,7 +10550,7 @@
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A177" s="106"/>
+      <c r="A177" s="108"/>
       <c r="B177" s="25"/>
       <c r="C177" s="19" t="s">
         <v>84</v>
@@ -10572,7 +10575,7 @@
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A178" s="106"/>
+      <c r="A178" s="108"/>
       <c r="B178" s="25"/>
       <c r="C178" s="19" t="s">
         <v>85</v>
@@ -10597,7 +10600,7 @@
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A179" s="106"/>
+      <c r="A179" s="108"/>
       <c r="B179" s="27" t="s">
         <v>95</v>
       </c>
@@ -10622,7 +10625,7 @@
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A180" s="106"/>
+      <c r="A180" s="108"/>
       <c r="B180" s="31"/>
       <c r="C180" s="14"/>
       <c r="D180" s="28" t="s">
@@ -10645,7 +10648,7 @@
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A181" s="106"/>
+      <c r="A181" s="108"/>
       <c r="B181" s="31"/>
       <c r="C181" s="14"/>
       <c r="D181" s="28" t="s">
@@ -10668,7 +10671,7 @@
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A182" s="106"/>
+      <c r="A182" s="108"/>
       <c r="B182" s="31"/>
       <c r="C182" s="19" t="s">
         <v>82</v>
@@ -10693,7 +10696,7 @@
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A183" s="106"/>
+      <c r="A183" s="108"/>
       <c r="B183" s="31"/>
       <c r="C183" s="19" t="s">
         <v>83</v>
@@ -10718,7 +10721,7 @@
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A184" s="106"/>
+      <c r="A184" s="108"/>
       <c r="B184" s="31"/>
       <c r="C184" s="19" t="s">
         <v>84</v>
@@ -10743,7 +10746,7 @@
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A185" s="106"/>
+      <c r="A185" s="108"/>
       <c r="B185" s="31"/>
       <c r="C185" s="19" t="s">
         <v>85</v>
@@ -10768,7 +10771,7 @@
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A186" s="106"/>
+      <c r="A186" s="108"/>
       <c r="B186" s="22" t="s">
         <v>116</v>
       </c>
@@ -10793,7 +10796,7 @@
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A187" s="106"/>
+      <c r="A187" s="108"/>
       <c r="B187" s="25"/>
       <c r="C187" s="14"/>
       <c r="D187" s="23" t="s">
@@ -10816,7 +10819,7 @@
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A188" s="106"/>
+      <c r="A188" s="108"/>
       <c r="B188" s="25"/>
       <c r="C188" s="14"/>
       <c r="D188" s="23" t="s">
@@ -10839,7 +10842,7 @@
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A189" s="106"/>
+      <c r="A189" s="108"/>
       <c r="B189" s="25"/>
       <c r="C189" s="19" t="s">
         <v>82</v>
@@ -10864,7 +10867,7 @@
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A190" s="106"/>
+      <c r="A190" s="108"/>
       <c r="B190" s="25"/>
       <c r="C190" s="19" t="s">
         <v>83</v>
@@ -10889,7 +10892,7 @@
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A191" s="106"/>
+      <c r="A191" s="108"/>
       <c r="B191" s="25"/>
       <c r="C191" s="19" t="s">
         <v>84</v>
@@ -10914,7 +10917,7 @@
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A192" s="106"/>
+      <c r="A192" s="108"/>
       <c r="B192" s="25"/>
       <c r="C192" s="19" t="s">
         <v>85</v>
@@ -10939,7 +10942,7 @@
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A193" s="106"/>
+      <c r="A193" s="108"/>
       <c r="B193" s="27" t="s">
         <v>117</v>
       </c>
@@ -10964,7 +10967,7 @@
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A194" s="106"/>
+      <c r="A194" s="108"/>
       <c r="B194" s="31"/>
       <c r="C194" s="14"/>
       <c r="D194" s="28" t="s">
@@ -10987,7 +10990,7 @@
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A195" s="106"/>
+      <c r="A195" s="108"/>
       <c r="B195" s="31"/>
       <c r="C195" s="14"/>
       <c r="D195" s="28" t="s">
@@ -11010,7 +11013,7 @@
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A196" s="106"/>
+      <c r="A196" s="108"/>
       <c r="B196" s="31"/>
       <c r="C196" s="19" t="s">
         <v>82</v>
@@ -11035,7 +11038,7 @@
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A197" s="106"/>
+      <c r="A197" s="108"/>
       <c r="B197" s="31"/>
       <c r="C197" s="19" t="s">
         <v>83</v>
@@ -11060,7 +11063,7 @@
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A198" s="106"/>
+      <c r="A198" s="108"/>
       <c r="B198" s="31"/>
       <c r="C198" s="19" t="s">
         <v>84</v>
@@ -11085,7 +11088,7 @@
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A199" s="106"/>
+      <c r="A199" s="108"/>
       <c r="B199" s="31"/>
       <c r="C199" s="19" t="s">
         <v>85</v>
@@ -11110,7 +11113,7 @@
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A200" s="106"/>
+      <c r="A200" s="108"/>
       <c r="B200" s="22" t="s">
         <v>119</v>
       </c>
@@ -11135,7 +11138,7 @@
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A201" s="106"/>
+      <c r="A201" s="108"/>
       <c r="B201" s="25"/>
       <c r="C201" s="14"/>
       <c r="D201" s="23" t="s">
@@ -11158,7 +11161,7 @@
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A202" s="106"/>
+      <c r="A202" s="108"/>
       <c r="B202" s="25"/>
       <c r="C202" s="14"/>
       <c r="D202" s="23" t="s">
@@ -11181,7 +11184,7 @@
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A203" s="106"/>
+      <c r="A203" s="108"/>
       <c r="B203" s="25"/>
       <c r="C203" s="19" t="s">
         <v>82</v>
@@ -11206,7 +11209,7 @@
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A204" s="106"/>
+      <c r="A204" s="108"/>
       <c r="B204" s="25"/>
       <c r="C204" s="19" t="s">
         <v>83</v>
@@ -11231,7 +11234,7 @@
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A205" s="106"/>
+      <c r="A205" s="108"/>
       <c r="B205" s="25"/>
       <c r="C205" s="19" t="s">
         <v>84</v>
@@ -11256,7 +11259,7 @@
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A206" s="106"/>
+      <c r="A206" s="108"/>
       <c r="B206" s="25"/>
       <c r="C206" s="19" t="s">
         <v>85</v>
@@ -11281,7 +11284,7 @@
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A207" s="106"/>
+      <c r="A207" s="108"/>
       <c r="B207" s="27" t="s">
         <v>120</v>
       </c>
@@ -11306,7 +11309,7 @@
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A208" s="106"/>
+      <c r="A208" s="108"/>
       <c r="B208" s="31"/>
       <c r="C208" s="14"/>
       <c r="D208" s="28" t="s">
@@ -11329,7 +11332,7 @@
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A209" s="106"/>
+      <c r="A209" s="108"/>
       <c r="B209" s="31"/>
       <c r="C209" s="14"/>
       <c r="D209" s="28" t="s">
@@ -11352,7 +11355,7 @@
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A210" s="106"/>
+      <c r="A210" s="108"/>
       <c r="B210" s="31"/>
       <c r="C210" s="19" t="s">
         <v>82</v>
@@ -11377,7 +11380,7 @@
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A211" s="106"/>
+      <c r="A211" s="108"/>
       <c r="B211" s="31"/>
       <c r="C211" s="19" t="s">
         <v>83</v>
@@ -11402,7 +11405,7 @@
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A212" s="106"/>
+      <c r="A212" s="108"/>
       <c r="B212" s="31"/>
       <c r="C212" s="19" t="s">
         <v>84</v>
@@ -11427,7 +11430,7 @@
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A213" s="106"/>
+      <c r="A213" s="108"/>
       <c r="B213" s="31"/>
       <c r="C213" s="19" t="s">
         <v>85</v>
@@ -11452,7 +11455,7 @@
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A214" s="106"/>
+      <c r="A214" s="108"/>
       <c r="B214" s="22" t="s">
         <v>123</v>
       </c>
@@ -11477,7 +11480,7 @@
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A215" s="106"/>
+      <c r="A215" s="108"/>
       <c r="B215" s="25"/>
       <c r="C215" s="14"/>
       <c r="D215" s="23" t="s">
@@ -11500,7 +11503,7 @@
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A216" s="106"/>
+      <c r="A216" s="108"/>
       <c r="B216" s="25"/>
       <c r="C216" s="14"/>
       <c r="D216" s="23" t="s">
@@ -11523,7 +11526,7 @@
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A217" s="106"/>
+      <c r="A217" s="108"/>
       <c r="B217" s="25"/>
       <c r="C217" s="19" t="s">
         <v>82</v>
@@ -11548,7 +11551,7 @@
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A218" s="106"/>
+      <c r="A218" s="108"/>
       <c r="B218" s="25"/>
       <c r="C218" s="19" t="s">
         <v>83</v>
@@ -11573,7 +11576,7 @@
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A219" s="106"/>
+      <c r="A219" s="108"/>
       <c r="B219" s="25"/>
       <c r="C219" s="19" t="s">
         <v>84</v>
@@ -11598,7 +11601,7 @@
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A220" s="106"/>
+      <c r="A220" s="108"/>
       <c r="B220" s="25"/>
       <c r="C220" s="19" t="s">
         <v>85</v>
@@ -11623,7 +11626,7 @@
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A221" s="106"/>
+      <c r="A221" s="108"/>
       <c r="B221" s="27" t="s">
         <v>128</v>
       </c>
@@ -11648,7 +11651,7 @@
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A222" s="106"/>
+      <c r="A222" s="108"/>
       <c r="B222" s="31"/>
       <c r="C222" s="14"/>
       <c r="D222" s="28" t="s">
@@ -11671,7 +11674,7 @@
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A223" s="106"/>
+      <c r="A223" s="108"/>
       <c r="B223" s="31"/>
       <c r="C223" s="14"/>
       <c r="D223" s="28" t="s">
@@ -11694,7 +11697,7 @@
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A224" s="106"/>
+      <c r="A224" s="108"/>
       <c r="B224" s="31"/>
       <c r="C224" s="19" t="s">
         <v>82</v>
@@ -11719,7 +11722,7 @@
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A225" s="106"/>
+      <c r="A225" s="108"/>
       <c r="B225" s="31"/>
       <c r="C225" s="19" t="s">
         <v>83</v>
@@ -11744,7 +11747,7 @@
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A226" s="106"/>
+      <c r="A226" s="108"/>
       <c r="B226" s="31"/>
       <c r="C226" s="19" t="s">
         <v>84</v>
@@ -11769,7 +11772,7 @@
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A227" s="106"/>
+      <c r="A227" s="108"/>
       <c r="B227" s="31"/>
       <c r="C227" s="19" t="s">
         <v>85</v>
@@ -11794,7 +11797,7 @@
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A228" s="111" t="s">
+      <c r="A228" s="113" t="s">
         <v>132</v>
       </c>
       <c r="B228" s="33" t="s">
@@ -11821,7 +11824,7 @@
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A229" s="112"/>
+      <c r="A229" s="114"/>
       <c r="B229" s="36"/>
       <c r="C229" s="14"/>
       <c r="D229" s="34" t="s">
@@ -11844,7 +11847,7 @@
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A230" s="112"/>
+      <c r="A230" s="114"/>
       <c r="B230" s="36"/>
       <c r="C230" s="14"/>
       <c r="D230" s="34" t="s">
@@ -11867,7 +11870,7 @@
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A231" s="112"/>
+      <c r="A231" s="114"/>
       <c r="B231" s="36"/>
       <c r="C231" s="19" t="s">
         <v>82</v>
@@ -11892,7 +11895,7 @@
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A232" s="112"/>
+      <c r="A232" s="114"/>
       <c r="B232" s="36"/>
       <c r="C232" s="19" t="s">
         <v>83</v>
@@ -11917,7 +11920,7 @@
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A233" s="112"/>
+      <c r="A233" s="114"/>
       <c r="B233" s="36"/>
       <c r="C233" s="19" t="s">
         <v>84</v>
@@ -11942,7 +11945,7 @@
       </c>
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A234" s="112"/>
+      <c r="A234" s="114"/>
       <c r="B234" s="36"/>
       <c r="C234" s="19" t="s">
         <v>85</v>
@@ -11967,7 +11970,7 @@
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A235" s="112"/>
+      <c r="A235" s="114"/>
       <c r="B235" s="37" t="s">
         <v>122</v>
       </c>
@@ -11992,7 +11995,7 @@
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A236" s="112"/>
+      <c r="A236" s="114"/>
       <c r="B236" s="40"/>
       <c r="C236" s="14"/>
       <c r="D236" s="38" t="s">
@@ -12015,7 +12018,7 @@
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A237" s="112"/>
+      <c r="A237" s="114"/>
       <c r="B237" s="40"/>
       <c r="C237" s="14"/>
       <c r="D237" s="38" t="s">
@@ -12038,7 +12041,7 @@
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A238" s="112"/>
+      <c r="A238" s="114"/>
       <c r="B238" s="40"/>
       <c r="C238" s="19" t="s">
         <v>82</v>
@@ -12063,7 +12066,7 @@
       </c>
     </row>
     <row r="239" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A239" s="112"/>
+      <c r="A239" s="114"/>
       <c r="B239" s="40"/>
       <c r="C239" s="19" t="s">
         <v>83</v>
@@ -12088,7 +12091,7 @@
       </c>
     </row>
     <row r="240" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A240" s="112"/>
+      <c r="A240" s="114"/>
       <c r="B240" s="40"/>
       <c r="C240" s="19" t="s">
         <v>84</v>
@@ -12113,7 +12116,7 @@
       </c>
     </row>
     <row r="241" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A241" s="112"/>
+      <c r="A241" s="114"/>
       <c r="B241" s="40"/>
       <c r="C241" s="19" t="s">
         <v>85</v>
@@ -12138,7 +12141,7 @@
       </c>
     </row>
     <row r="242" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A242" s="112"/>
+      <c r="A242" s="114"/>
       <c r="B242" s="33" t="s">
         <v>95</v>
       </c>
@@ -12163,7 +12166,7 @@
       </c>
     </row>
     <row r="243" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A243" s="112"/>
+      <c r="A243" s="114"/>
       <c r="B243" s="36"/>
       <c r="C243" s="14"/>
       <c r="D243" s="34" t="s">
@@ -12186,7 +12189,7 @@
       </c>
     </row>
     <row r="244" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A244" s="112"/>
+      <c r="A244" s="114"/>
       <c r="B244" s="36"/>
       <c r="C244" s="14"/>
       <c r="D244" s="34" t="s">
@@ -12209,7 +12212,7 @@
       </c>
     </row>
     <row r="245" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A245" s="112"/>
+      <c r="A245" s="114"/>
       <c r="B245" s="36"/>
       <c r="C245" s="19" t="s">
         <v>82</v>
@@ -12234,7 +12237,7 @@
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A246" s="112"/>
+      <c r="A246" s="114"/>
       <c r="B246" s="36"/>
       <c r="C246" s="19" t="s">
         <v>83</v>
@@ -12259,7 +12262,7 @@
       </c>
     </row>
     <row r="247" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A247" s="112"/>
+      <c r="A247" s="114"/>
       <c r="B247" s="36"/>
       <c r="C247" s="19" t="s">
         <v>84</v>
@@ -12284,7 +12287,7 @@
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A248" s="112"/>
+      <c r="A248" s="114"/>
       <c r="B248" s="36"/>
       <c r="C248" s="19" t="s">
         <v>85</v>
@@ -12309,7 +12312,7 @@
       </c>
     </row>
     <row r="249" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A249" s="112"/>
+      <c r="A249" s="114"/>
       <c r="B249" s="37" t="s">
         <v>121</v>
       </c>
@@ -12334,7 +12337,7 @@
       </c>
     </row>
     <row r="250" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A250" s="112"/>
+      <c r="A250" s="114"/>
       <c r="B250" s="40"/>
       <c r="C250" s="14"/>
       <c r="D250" s="38" t="s">
@@ -12357,7 +12360,7 @@
       </c>
     </row>
     <row r="251" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A251" s="112"/>
+      <c r="A251" s="114"/>
       <c r="B251" s="40"/>
       <c r="C251" s="14"/>
       <c r="D251" s="38" t="s">
@@ -12380,7 +12383,7 @@
       </c>
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A252" s="112"/>
+      <c r="A252" s="114"/>
       <c r="B252" s="40"/>
       <c r="C252" s="19" t="s">
         <v>82</v>
@@ -12405,7 +12408,7 @@
       </c>
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A253" s="112"/>
+      <c r="A253" s="114"/>
       <c r="B253" s="40"/>
       <c r="C253" s="19" t="s">
         <v>83</v>
@@ -12430,7 +12433,7 @@
       </c>
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A254" s="112"/>
+      <c r="A254" s="114"/>
       <c r="B254" s="40"/>
       <c r="C254" s="19" t="s">
         <v>84</v>
@@ -12455,7 +12458,7 @@
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A255" s="112"/>
+      <c r="A255" s="114"/>
       <c r="B255" s="40"/>
       <c r="C255" s="19" t="s">
         <v>85</v>
@@ -12480,7 +12483,7 @@
       </c>
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A256" s="112"/>
+      <c r="A256" s="114"/>
       <c r="B256" s="33" t="s">
         <v>116</v>
       </c>
@@ -12505,7 +12508,7 @@
       </c>
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A257" s="112"/>
+      <c r="A257" s="114"/>
       <c r="B257" s="36"/>
       <c r="C257" s="14"/>
       <c r="D257" s="34" t="s">
@@ -12528,7 +12531,7 @@
       </c>
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A258" s="112"/>
+      <c r="A258" s="114"/>
       <c r="B258" s="36"/>
       <c r="C258" s="14"/>
       <c r="D258" s="34" t="s">
@@ -12551,7 +12554,7 @@
       </c>
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A259" s="112"/>
+      <c r="A259" s="114"/>
       <c r="B259" s="36"/>
       <c r="C259" s="19" t="s">
         <v>82</v>
@@ -12576,7 +12579,7 @@
       </c>
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A260" s="112"/>
+      <c r="A260" s="114"/>
       <c r="B260" s="36"/>
       <c r="C260" s="19" t="s">
         <v>83</v>
@@ -12601,7 +12604,7 @@
       </c>
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A261" s="112"/>
+      <c r="A261" s="114"/>
       <c r="B261" s="36"/>
       <c r="C261" s="19" t="s">
         <v>84</v>
@@ -12626,7 +12629,7 @@
       </c>
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A262" s="112"/>
+      <c r="A262" s="114"/>
       <c r="B262" s="36"/>
       <c r="C262" s="19" t="s">
         <v>85</v>
@@ -12651,7 +12654,7 @@
       </c>
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A263" s="112"/>
+      <c r="A263" s="114"/>
       <c r="B263" s="37" t="s">
         <v>117</v>
       </c>
@@ -12676,7 +12679,7 @@
       </c>
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A264" s="112"/>
+      <c r="A264" s="114"/>
       <c r="B264" s="40"/>
       <c r="C264" s="14"/>
       <c r="D264" s="38" t="s">
@@ -12699,7 +12702,7 @@
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A265" s="112"/>
+      <c r="A265" s="114"/>
       <c r="B265" s="40"/>
       <c r="C265" s="14"/>
       <c r="D265" s="38" t="s">
@@ -12722,7 +12725,7 @@
       </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A266" s="112"/>
+      <c r="A266" s="114"/>
       <c r="B266" s="40"/>
       <c r="C266" s="19" t="s">
         <v>82</v>
@@ -12747,7 +12750,7 @@
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A267" s="112"/>
+      <c r="A267" s="114"/>
       <c r="B267" s="40"/>
       <c r="C267" s="19" t="s">
         <v>83</v>
@@ -12772,7 +12775,7 @@
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A268" s="112"/>
+      <c r="A268" s="114"/>
       <c r="B268" s="40"/>
       <c r="C268" s="19" t="s">
         <v>84</v>
@@ -12797,7 +12800,7 @@
       </c>
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A269" s="112"/>
+      <c r="A269" s="114"/>
       <c r="B269" s="40"/>
       <c r="C269" s="19" t="s">
         <v>85</v>
@@ -12822,7 +12825,7 @@
       </c>
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A270" s="112"/>
+      <c r="A270" s="114"/>
       <c r="B270" s="33" t="s">
         <v>119</v>
       </c>
@@ -12847,7 +12850,7 @@
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A271" s="112"/>
+      <c r="A271" s="114"/>
       <c r="B271" s="36"/>
       <c r="C271" s="14"/>
       <c r="D271" s="34" t="s">
@@ -12870,7 +12873,7 @@
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A272" s="112"/>
+      <c r="A272" s="114"/>
       <c r="B272" s="36"/>
       <c r="C272" s="14"/>
       <c r="D272" s="34" t="s">
@@ -12893,7 +12896,7 @@
       </c>
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A273" s="112"/>
+      <c r="A273" s="114"/>
       <c r="B273" s="36"/>
       <c r="C273" s="19" t="s">
         <v>82</v>
@@ -12918,7 +12921,7 @@
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A274" s="112"/>
+      <c r="A274" s="114"/>
       <c r="B274" s="36"/>
       <c r="C274" s="19" t="s">
         <v>83</v>
@@ -12943,7 +12946,7 @@
       </c>
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A275" s="112"/>
+      <c r="A275" s="114"/>
       <c r="B275" s="36"/>
       <c r="C275" s="19" t="s">
         <v>84</v>
@@ -12968,7 +12971,7 @@
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A276" s="112"/>
+      <c r="A276" s="114"/>
       <c r="B276" s="36"/>
       <c r="C276" s="19" t="s">
         <v>85</v>
@@ -12993,7 +12996,7 @@
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A277" s="112"/>
+      <c r="A277" s="114"/>
       <c r="B277" s="37" t="s">
         <v>120</v>
       </c>
@@ -13018,7 +13021,7 @@
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A278" s="112"/>
+      <c r="A278" s="114"/>
       <c r="B278" s="40"/>
       <c r="C278" s="14"/>
       <c r="D278" s="38" t="s">
@@ -13041,7 +13044,7 @@
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A279" s="112"/>
+      <c r="A279" s="114"/>
       <c r="B279" s="40"/>
       <c r="C279" s="14"/>
       <c r="D279" s="38" t="s">
@@ -13064,7 +13067,7 @@
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A280" s="112"/>
+      <c r="A280" s="114"/>
       <c r="B280" s="40"/>
       <c r="C280" s="19" t="s">
         <v>82</v>
@@ -13089,7 +13092,7 @@
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A281" s="112"/>
+      <c r="A281" s="114"/>
       <c r="B281" s="40"/>
       <c r="C281" s="19" t="s">
         <v>83</v>
@@ -13114,7 +13117,7 @@
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A282" s="112"/>
+      <c r="A282" s="114"/>
       <c r="B282" s="40"/>
       <c r="C282" s="19" t="s">
         <v>84</v>
@@ -13139,7 +13142,7 @@
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A283" s="112"/>
+      <c r="A283" s="114"/>
       <c r="B283" s="40"/>
       <c r="C283" s="19" t="s">
         <v>85</v>
@@ -13164,7 +13167,7 @@
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A284" s="112"/>
+      <c r="A284" s="114"/>
       <c r="B284" s="33" t="s">
         <v>123</v>
       </c>
@@ -13189,7 +13192,7 @@
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A285" s="112"/>
+      <c r="A285" s="114"/>
       <c r="B285" s="36"/>
       <c r="C285" s="14"/>
       <c r="D285" s="34" t="s">
@@ -13212,7 +13215,7 @@
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A286" s="112"/>
+      <c r="A286" s="114"/>
       <c r="B286" s="36"/>
       <c r="C286" s="14"/>
       <c r="D286" s="34" t="s">
@@ -13235,7 +13238,7 @@
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A287" s="112"/>
+      <c r="A287" s="114"/>
       <c r="B287" s="36"/>
       <c r="C287" s="19" t="s">
         <v>82</v>
@@ -13260,7 +13263,7 @@
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A288" s="112"/>
+      <c r="A288" s="114"/>
       <c r="B288" s="36"/>
       <c r="C288" s="19" t="s">
         <v>83</v>
@@ -13285,7 +13288,7 @@
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A289" s="112"/>
+      <c r="A289" s="114"/>
       <c r="B289" s="36"/>
       <c r="C289" s="19" t="s">
         <v>84</v>
@@ -13310,7 +13313,7 @@
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A290" s="112"/>
+      <c r="A290" s="114"/>
       <c r="B290" s="36"/>
       <c r="C290" s="19" t="s">
         <v>85</v>
@@ -13335,7 +13338,7 @@
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A291" s="112"/>
+      <c r="A291" s="114"/>
       <c r="B291" s="37" t="s">
         <v>128</v>
       </c>
@@ -13360,7 +13363,7 @@
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A292" s="112"/>
+      <c r="A292" s="114"/>
       <c r="B292" s="40"/>
       <c r="C292" s="14"/>
       <c r="D292" s="38" t="s">
@@ -13383,7 +13386,7 @@
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A293" s="112"/>
+      <c r="A293" s="114"/>
       <c r="B293" s="40"/>
       <c r="C293" s="14"/>
       <c r="D293" s="38" t="s">
@@ -13406,7 +13409,7 @@
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A294" s="112"/>
+      <c r="A294" s="114"/>
       <c r="B294" s="40"/>
       <c r="C294" s="19" t="s">
         <v>82</v>
@@ -13431,7 +13434,7 @@
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A295" s="112"/>
+      <c r="A295" s="114"/>
       <c r="B295" s="40"/>
       <c r="C295" s="19" t="s">
         <v>83</v>
@@ -13456,7 +13459,7 @@
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A296" s="112"/>
+      <c r="A296" s="114"/>
       <c r="B296" s="40"/>
       <c r="C296" s="19" t="s">
         <v>84</v>
@@ -13481,7 +13484,7 @@
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A297" s="112"/>
+      <c r="A297" s="114"/>
       <c r="B297" s="40"/>
       <c r="C297" s="19" t="s">
         <v>85</v>
@@ -13506,7 +13509,7 @@
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A298" s="105" t="s">
+      <c r="A298" s="107" t="s">
         <v>133</v>
       </c>
       <c r="B298" s="22" t="s">
@@ -13533,7 +13536,7 @@
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A299" s="106"/>
+      <c r="A299" s="108"/>
       <c r="B299" s="25"/>
       <c r="C299" s="14"/>
       <c r="D299" s="23" t="s">
@@ -13556,7 +13559,7 @@
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A300" s="106"/>
+      <c r="A300" s="108"/>
       <c r="B300" s="25"/>
       <c r="C300" s="14"/>
       <c r="D300" s="23" t="s">
@@ -13579,7 +13582,7 @@
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A301" s="106"/>
+      <c r="A301" s="108"/>
       <c r="B301" s="25"/>
       <c r="C301" s="19" t="s">
         <v>82</v>
@@ -13604,7 +13607,7 @@
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A302" s="106"/>
+      <c r="A302" s="108"/>
       <c r="B302" s="25"/>
       <c r="C302" s="19" t="s">
         <v>83</v>
@@ -13629,7 +13632,7 @@
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A303" s="106"/>
+      <c r="A303" s="108"/>
       <c r="B303" s="25"/>
       <c r="C303" s="19" t="s">
         <v>84</v>
@@ -13654,7 +13657,7 @@
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A304" s="106"/>
+      <c r="A304" s="108"/>
       <c r="B304" s="25"/>
       <c r="C304" s="19" t="s">
         <v>85</v>
@@ -13679,7 +13682,7 @@
       </c>
     </row>
     <row r="305" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A305" s="106"/>
+      <c r="A305" s="108"/>
       <c r="B305" s="27" t="s">
         <v>124</v>
       </c>
@@ -13704,7 +13707,7 @@
       </c>
     </row>
     <row r="306" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A306" s="106"/>
+      <c r="A306" s="108"/>
       <c r="B306" s="31"/>
       <c r="C306" s="14"/>
       <c r="D306" s="28" t="s">
@@ -13727,7 +13730,7 @@
       </c>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A307" s="106"/>
+      <c r="A307" s="108"/>
       <c r="B307" s="31"/>
       <c r="C307" s="14"/>
       <c r="D307" s="28" t="s">
@@ -13750,7 +13753,7 @@
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A308" s="106"/>
+      <c r="A308" s="108"/>
       <c r="B308" s="31"/>
       <c r="C308" s="19" t="s">
         <v>82</v>
@@ -13775,7 +13778,7 @@
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A309" s="106"/>
+      <c r="A309" s="108"/>
       <c r="B309" s="31"/>
       <c r="C309" s="19" t="s">
         <v>83</v>
@@ -13800,7 +13803,7 @@
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A310" s="106"/>
+      <c r="A310" s="108"/>
       <c r="B310" s="31"/>
       <c r="C310" s="19" t="s">
         <v>84</v>
@@ -13825,7 +13828,7 @@
       </c>
     </row>
     <row r="311" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A311" s="106"/>
+      <c r="A311" s="108"/>
       <c r="B311" s="31"/>
       <c r="C311" s="19" t="s">
         <v>85</v>

</xml_diff>